<commit_message>
Fix columns to line up exactly with the XML document.
</commit_message>
<xml_diff>
--- a/tests/data/fagatelebay.xlsx
+++ b/tests/data/fagatelebay.xlsx
@@ -443,7 +443,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="C11">
         <v>100</v>
       </c>
       <c r="F11">
@@ -685,7 +685,7 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="D12">
+      <c r="C12">
         <v>100</v>
       </c>
       <c r="E12">

</xml_diff>